<commit_message>
refresh app color palette with new theme
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -416,13 +416,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Rent</v>
+        <v>ferrari</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C2" s="1">
-        <v>45778.083333333336</v>
+        <v>46325.041666666664</v>
       </c>
     </row>
     <row r="3">
@@ -430,32 +430,32 @@
         <v>Food</v>
       </c>
       <c r="B3">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="C3" s="1">
-        <v>45748.083333333336</v>
+        <v>46138.083333333336</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v xml:space="preserve">Stock: Ethereum </v>
+        <v>But business with bestfriendo</v>
       </c>
       <c r="B4">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="C4" s="1">
-        <v>45415.083333333336</v>
+        <v>45935.083333333336</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Fuel</v>
+        <v>food</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C5" s="1">
-        <v>-685098.9604166667</v>
+        <v>45930.083333333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>